<commit_message>
Added test cases for task 1. Added picture for the task 1.
</commit_message>
<xml_diff>
--- a/Test cases/Test Cases_ 1.xlsx
+++ b/Test cases/Test Cases_ 1.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Task" sheetId="1" r:id="rId1"/>
+    <sheet name="Search field" sheetId="2" r:id="rId2"/>
+    <sheet name="Search results" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="90">
   <si>
     <t>Search field:</t>
   </si>
@@ -46,13 +48,308 @@
   </si>
   <si>
     <t>Написать 5 test cases для Search и 5 test cases для Search results.</t>
+  </si>
+  <si>
+    <t>User Story/ Requirement link</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Test ID</t>
+  </si>
+  <si>
+    <t>Pre-conditions</t>
+  </si>
+  <si>
+    <t>Test Name (Objective)</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Link to Bug</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Exectutor</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Time spent(min)</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>Windows 7, Google Chrome v.92.0.4515.107</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>The user can enter letters in the search field</t>
+  </si>
+  <si>
+    <t>Pass/Fail/Blocked</t>
+  </si>
+  <si>
+    <t>Alina Paliakova</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>The site page is loading</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Click on the search field</t>
+  </si>
+  <si>
+    <t>The input cursor appears in the search field</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>Enter letters in the search field</t>
+  </si>
+  <si>
+    <t>The letters are displayed in the search field</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>The user can enter numbers in the search field</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>Enter numbers in the search field</t>
+  </si>
+  <si>
+    <t>The numbers are displayed in the search field</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>You are went to https://www.search.com/ and clicked on the search field</t>
+  </si>
+  <si>
+    <t>The user can enter a phrase with a length of 40 characters</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter a phrase with a length of 40 characters in the search field </t>
+  </si>
+  <si>
+    <t>The phrase with a length of 40 characters is displayed in the search field</t>
+  </si>
+  <si>
+    <t>You can use www.blindtextgenerator.com to generate text</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>Enter a phrase with a length of 40 characters using CTRL+V in the search field</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>The user can't enter a phrase more than with a length of 40 characters</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>Enter a phrase more than with a length of 40 characters in the search field</t>
+  </si>
+  <si>
+    <t>Only the first 40 characters are displayed in the search field</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>Enter a phrase more than with a length of 40 characters using CTRL+V in the search field</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user can go to the search results page after clicking the button "search" </t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>Enter a valid search term in the search field (e.g.sunset photos)</t>
+  </si>
+  <si>
+    <t>The search term is displayed in the search field</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>Click on the button "search"</t>
+  </si>
+  <si>
+    <t>The search results page is loading</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Go to  </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://www.search.com/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">You are went to </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://www.search.com/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and clicked on the search field</t>
+    </r>
+  </si>
+  <si>
+    <t>You are went to https://www.search.com/, clicked on the search field and enter a search term in the search field</t>
+  </si>
+  <si>
+    <t>The search results are relevant</t>
+  </si>
+  <si>
+    <t>Relevant search results are displayed on the search results page</t>
+  </si>
+  <si>
+    <t>The search results are displayed in the list format</t>
+  </si>
+  <si>
+    <t>The search results page is displayed in the list format</t>
+  </si>
+  <si>
+    <t>The user can use the page scroll bar</t>
+  </si>
+  <si>
+    <t>Use the page scroll bar</t>
+  </si>
+  <si>
+    <t>The page moves up and down</t>
+  </si>
+  <si>
+    <t>The user can go to the next page of search results</t>
+  </si>
+  <si>
+    <t>Scroll down the page</t>
+  </si>
+  <si>
+    <t>Go to the bottom of the search page</t>
+  </si>
+  <si>
+    <t>Сlick on the button numbers of the next search results page</t>
+  </si>
+  <si>
+    <t>Go to the next page of search results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The message "No results found for this term" is displayed on the search results page </t>
+  </si>
+  <si>
+    <t>The user can see a message "No results found for this term" when performing a search if there aren't  results for this query</t>
+  </si>
+  <si>
+    <t>5.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,8 +364,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF1155CC"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -87,8 +426,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7F4EC"/>
+        <bgColor rgb="FFF7F4EC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFF7F4EC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -111,11 +468,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -123,11 +508,76 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -144,6 +594,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1895476</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1211513</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1352550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1895476" y="2476500"/>
+          <a:ext cx="2506912" cy="1276350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -409,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,16 +921,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="17"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -463,11 +962,963 @@
       </c>
       <c r="B6" s="2"/>
     </row>
+    <row r="7" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+    </row>
+    <row r="6" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+    </row>
+    <row r="8" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N8" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+    </row>
+    <row r="10" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N14" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="D6" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+    </row>
+    <row r="4" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+    </row>
+    <row r="6" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+    </row>
+    <row r="8" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="N8" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+    </row>
+    <row r="10" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+    </row>
+    <row r="11" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+    </row>
+    <row r="12" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+    </row>
+    <row r="14" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>